<commit_message>
📊 OLX Monitor 2026-02-15 21:17
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -100,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -133,6 +133,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -558,7 +561,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 20:58</t>
+          <t>2026-02-15 21:16</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
@@ -584,7 +587,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 20:58</t>
+          <t>2026-02-15 21:16</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -610,14 +613,14 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 20:58</t>
+          <t>2026-02-15 21:16</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
         <v>5</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>0</v>
@@ -636,14 +639,14 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 20:58</t>
+          <t>2026-02-15 21:16</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>0</v>
@@ -662,7 +665,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 20:58</t>
+          <t>2026-02-15 21:16</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -691,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -786,7 +789,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3" ht="18" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:16</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>431</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -799,7 +836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -894,7 +931,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3" ht="18" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:16</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -907,7 +978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1008,6 +1079,45 @@
         </is>
       </c>
     </row>
+    <row r="3" ht="18" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:16</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>18KAEc|183ger|17NeTz|1951OR|17vbYq</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1019,7 +1129,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1120,6 +1230,45 @@
         </is>
       </c>
     </row>
+    <row r="3" ht="18" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:16</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>16ZeYm|195dLc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1131,7 +1280,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1226,7 +1375,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3" ht="18" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:16</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-15 21:48
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -561,13 +561,13 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:16</t>
+          <t>2026-02-15 21:47</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>431</v>
-      </c>
-      <c r="D2" s="4" t="n">
+        <v>432</v>
+      </c>
+      <c r="D2" s="6" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="4" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:16</t>
+          <t>2026-02-15 21:47</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -613,7 +613,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:16</t>
+          <t>2026-02-15 21:47</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -639,7 +639,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:16</t>
+          <t>2026-02-15 21:47</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -665,7 +665,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:16</t>
+          <t>2026-02-15 21:47</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -694,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -823,7 +823,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>432</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>432</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -836,7 +904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -965,7 +1033,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -978,7 +1114,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1118,6 +1254,84 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>17NeTz|18KAEc|183ger|1951OR|17vbYq</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>17vbYq|17NeTz|183ger|1951OR|18KAEc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1129,7 +1343,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1269,6 +1483,84 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>16ZeYm|195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>195dLc|16ZeYm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1280,7 +1572,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1409,7 +1701,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:47</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-15 21:52
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:47</t>
+          <t>2026-02-15 21:51</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:47</t>
+          <t>2026-02-15 21:51</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -613,7 +613,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:47</t>
+          <t>2026-02-15 21:51</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -639,7 +639,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:47</t>
+          <t>2026-02-15 21:51</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -665,7 +665,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:47</t>
+          <t>2026-02-15 21:51</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -694,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -891,7 +891,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>432</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>432</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -904,7 +972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1101,7 +1169,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1114,7 +1250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1332,6 +1468,84 @@
         </is>
       </c>
     </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>1951OR|17NeTz|17vbYq|18KAEc|183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>183ger|18KAEc|17NeTz|17vbYq|1951OR</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1343,7 +1557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1561,6 +1775,84 @@
         </is>
       </c>
     </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>195dLc|16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>16ZeYm|195dLc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1572,7 +1864,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1769,7 +2061,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:51</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G7" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-15 21:59
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:51</t>
+          <t>2026-02-15 21:59</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:51</t>
+          <t>2026-02-15 21:59</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -613,7 +613,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:51</t>
+          <t>2026-02-15 21:59</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -639,7 +639,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:51</t>
+          <t>2026-02-15 21:59</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -665,7 +665,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:51</t>
+          <t>2026-02-15 21:59</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -694,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -959,7 +959,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:58</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>432</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:59</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>432</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -972,7 +1040,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1237,7 +1305,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:58</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:59</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1250,7 +1386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1546,6 +1682,84 @@
         </is>
       </c>
     </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:58</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>18KAEc|17vbYq|1951OR|17NeTz|183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:59</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1951OR|17NeTz|17vbYq|183ger|18KAEc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1557,7 +1771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1853,6 +2067,84 @@
         </is>
       </c>
     </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:58</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>16ZeYm|195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:59</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>16ZeYm|195dLc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1864,7 +2156,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2129,7 +2421,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:58</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 21:59</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G9" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-15 22:01
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:59</t>
+          <t>2026-02-15 22:01</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:59</t>
+          <t>2026-02-15 22:01</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -613,7 +613,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:59</t>
+          <t>2026-02-15 22:01</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -639,7 +639,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:59</t>
+          <t>2026-02-15 22:01</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -665,7 +665,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 21:59</t>
+          <t>2026-02-15 22:01</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -694,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1027,7 +1027,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>432</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>432</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1040,7 +1108,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1373,7 +1441,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1386,7 +1522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1760,6 +1896,84 @@
         </is>
       </c>
     </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>183ger|18KAEc|17NeTz|17vbYq|1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>17vbYq|17NeTz|183ger|18KAEc|1951OR</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1771,7 +1985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2145,6 +2359,84 @@
         </is>
       </c>
     </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>195dLc|16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>195dLc|16ZeYm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2156,7 +2448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2489,7 +2781,75 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G10" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:01</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G11" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-15 22:05
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:01</t>
+          <t>2026-02-15 22:05</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:01</t>
+          <t>2026-02-15 22:05</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -613,7 +613,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:01</t>
+          <t>2026-02-15 22:05</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -639,7 +639,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:01</t>
+          <t>2026-02-15 22:05</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -665,7 +665,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:01</t>
+          <t>2026-02-15 22:05</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -694,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1095,7 +1095,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:05</t>
+        </is>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>432</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1108,7 +1142,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1509,7 +1543,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:05</t>
+        </is>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1522,7 +1590,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1974,6 +2042,45 @@
         </is>
       </c>
     </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:05</t>
+        </is>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1951OR|183ger|17NeTz|17vbYq|18KAEc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1985,7 +2092,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2437,6 +2544,45 @@
         </is>
       </c>
     </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:05</t>
+        </is>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>195dLc|16ZeYm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2448,7 +2594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2849,7 +2995,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:05</t>
+        </is>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-15 22:07
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:05</t>
+          <t>2026-02-15 22:07</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:05</t>
+          <t>2026-02-15 22:07</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -613,7 +613,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:05</t>
+          <t>2026-02-15 22:07</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -639,7 +639,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:05</t>
+          <t>2026-02-15 22:07</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -665,7 +665,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:05</t>
+          <t>2026-02-15 22:07</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -694,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1129,7 +1129,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13" ht="18" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:07</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>432</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1142,7 +1176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1577,7 +1611,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13" ht="18" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:07</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1590,7 +1658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2081,6 +2149,45 @@
         </is>
       </c>
     </row>
+    <row r="13" ht="18" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:07</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1951OR|17NeTz|17vbYq|18KAEc|183ger</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2092,7 +2199,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2583,6 +2690,45 @@
         </is>
       </c>
     </row>
+    <row r="13" ht="18" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:07</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>195dLc|16ZeYm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2594,7 +2740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3029,7 +3175,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13" ht="18" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-15 22:07</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G13" s="12" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-16 09:39
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -561,14 +561,14 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:07</t>
+          <t>2026-02-16 09:38</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>0</v>
@@ -587,7 +587,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:07</t>
+          <t>2026-02-16 09:38</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
@@ -613,7 +613,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:07</t>
+          <t>2026-02-16 09:38</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -639,7 +639,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:07</t>
+          <t>2026-02-16 09:38</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -665,7 +665,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2026-02-15 22:07</t>
+          <t>2026-02-16 09:38</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -694,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1163,7 +1163,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-16 09:38</t>
+        </is>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>434</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="11" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1176,7 +1210,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1645,7 +1679,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-16 09:38</t>
+        </is>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1658,7 +1726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2188,6 +2256,45 @@
         </is>
       </c>
     </row>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-16 09:38</t>
+        </is>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1951OR|183ger|17vbYq|17NeTz|18KAEc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2199,7 +2306,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2729,6 +2836,45 @@
         </is>
       </c>
     </row>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-16 09:38</t>
+        </is>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>195dLc|16ZeYm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2740,7 +2886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3209,7 +3355,41 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>2026-02-16 09:38</t>
+        </is>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-17 11:35
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -43,6 +43,10 @@
     </font>
     <font>
       <name val="Arial"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <color rgb="00ff6b6b"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -100,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -137,6 +141,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -680,6 +693,310 @@
       <c r="F6" s="5" t="inlineStr">
         <is>
           <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:35:18</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C7" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D7" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E7" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F7" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:35:18</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C8" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E8" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F8" s="15" t="n">
+        <v>111</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:35:18</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C9" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D9" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E9" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F9" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:35:18</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C10" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D10" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E10" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F10" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:35:18</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C11" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D11" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E11" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F11" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:35:18</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C12" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D12" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E12" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F12" s="14" t="n">
+        <v>28</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:35:18</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C13" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F13" s="15" t="n">
+        <v>514</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:35:18</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C14" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F14" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1514,6 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1713,7 +2029,6 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3389,7 +3704,6 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-17 11:36
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1000,6 +1000,310 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:36:19</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C15" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D15" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E15" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F15" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:36:19</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C16" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D16" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E16" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F16" s="15" t="n">
+        <v>111</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:36:19</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C17" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D17" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E17" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F17" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:36:19</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C18" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D18" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E18" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F18" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:36:19</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C19" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D19" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E19" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F19" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:36:19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C20" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D20" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E20" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F20" s="14" t="n">
+        <v>28</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:36:19</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C21" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D21" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E21" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F21" s="15" t="n">
+        <v>514</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 11:36:19</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C22" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D22" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E22" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F22" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1011,7 +1315,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1526,7 +1830,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3201,7 +3505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-17 12:01
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1299,6 +1299,310 @@
         </is>
       </c>
       <c r="H22" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 12:01:39</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C23" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D23" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E23" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F23" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 12:01:39</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C24" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D24" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E24" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F24" s="15" t="n">
+        <v>111</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 12:01:39</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C25" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D25" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E25" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F25" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 12:01:39</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C26" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D26" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E26" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F26" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 12:01:39</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C27" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D27" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E27" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F27" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 12:01:39</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C28" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D28" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E28" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F28" s="14" t="n">
+        <v>28</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 12:01:39</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C29" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D29" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E29" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F29" s="15" t="n">
+        <v>514</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 12:01:39</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C30" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D30" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E30" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F30" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-17 13:19
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1603,6 +1603,310 @@
         </is>
       </c>
       <c r="H30" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:19:00</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C31" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D31" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E31" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F31" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:19:00</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C32" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D32" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E32" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F32" s="15" t="n">
+        <v>111</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:19:00</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C33" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D33" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E33" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F33" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:19:00</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C34" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D34" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E34" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F34" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:19:00</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C35" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D35" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E35" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F35" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:19:00</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C36" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D36" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E36" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F36" s="14" t="n">
+        <v>28</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:19:00</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C37" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D37" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E37" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F37" s="15" t="n">
+        <v>515</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:19:00</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C38" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D38" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E38" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F38" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-17 14:21
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1907,6 +1907,310 @@
         </is>
       </c>
       <c r="H38" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:21:01</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C39" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D39" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E39" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F39" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:21:01</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C40" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D40" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E40" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F40" s="15" t="n">
+        <v>111</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:21:01</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C41" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D41" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E41" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F41" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:21:01</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C42" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D42" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E42" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F42" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:21:01</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C43" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D43" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E43" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F43" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:21:01</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C44" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D44" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E44" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F44" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:21:01</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C45" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D45" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E45" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F45" s="15" t="n">
+        <v>515</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:21:01</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C46" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D46" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E46" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F46" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-17 16:33
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2211,6 +2211,272 @@
         </is>
       </c>
       <c r="H46" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 16:33:37</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C47" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D47" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E47" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F47" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 16:33:37</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C48" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D48" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E48" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F48" s="15" t="n">
+        <v>112</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 16:33:37</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C49" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D49" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E49" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F49" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 16:33:37</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C50" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D50" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E50" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F50" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 16:33:37</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C51" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D51" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E51" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F51" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 16:33:37</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C52" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D52" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E52" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F52" s="15" t="n">
+        <v>515</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 16:33:37</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C53" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D53" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E53" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F53" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-17 17:05
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2477,6 +2477,272 @@
         </is>
       </c>
       <c r="H53" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 17:05:28</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C54" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D54" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E54" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F54" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 17:05:28</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C55" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D55" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E55" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F55" s="15" t="n">
+        <v>112</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 17:05:28</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C56" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D56" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E56" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F56" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 17:05:28</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C57" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D57" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E57" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F57" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 17:05:28</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C58" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D58" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E58" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F58" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 17:05:28</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C59" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D59" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E59" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F59" s="15" t="n">
+        <v>515</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 17:05:28</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C60" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D60" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E60" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F60" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-17 18:21
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2743,6 +2743,272 @@
         </is>
       </c>
       <c r="H60" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 18:21:25</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C61" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D61" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E61" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F61" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 18:21:25</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C62" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D62" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E62" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F62" s="15" t="n">
+        <v>112</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 18:21:25</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C63" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D63" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E63" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F63" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 18:21:25</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C64" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D64" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E64" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F64" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 18:21:25</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C65" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D65" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E65" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F65" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 18:21:25</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C66" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D66" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E66" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F66" s="15" t="n">
+        <v>515</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-17 18:21:25</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C67" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D67" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E67" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F67" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-18 09:33
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3009,6 +3009,272 @@
         </is>
       </c>
       <c r="H67" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-18 09:33:13</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C68" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D68" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E68" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F68" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-18 09:33:13</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C69" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D69" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E69" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F69" s="15" t="n">
+        <v>112</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-18 09:33:13</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C70" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D70" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E70" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F70" s="15" t="n">
+        <v>131</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-18 09:33:13</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C71" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D71" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E71" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F71" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-18 09:33:13</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C72" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D72" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E72" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F72" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-18 09:33:13</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C73" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D73" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E73" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F73" s="15" t="n">
+        <v>515</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-18 09:33:13</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C74" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D74" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E74" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F74" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-19 08:46
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3275,6 +3275,310 @@
         </is>
       </c>
       <c r="H74" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 08:46:44</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C75" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D75" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E75" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F75" s="15" t="n">
+        <v>113</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 08:46:44</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C76" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D76" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E76" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F76" s="14" t="n">
+        <v>30</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 08:46:44</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C77" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D77" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E77" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F77" s="15" t="n">
+        <v>61</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 08:46:44</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C78" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D78" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E78" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F78" s="15" t="n">
+        <v>131</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 08:46:44</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C79" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D79" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E79" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F79" s="15" t="n">
+        <v>191</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 08:46:44</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C80" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D80" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E80" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F80" s="14" t="n">
+        <v>30</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 08:46:44</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C81" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D81" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E81" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F81" s="15" t="n">
+        <v>516</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 08:46:44</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C82" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D82" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E82" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F82" s="15" t="n">
+        <v>75</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-19 09:32
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3579,6 +3579,310 @@
         </is>
       </c>
       <c r="H82" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 09:32:21</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C83" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D83" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E83" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F83" s="15" t="n">
+        <v>113</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 09:32:21</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C84" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D84" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E84" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F84" s="14" t="n">
+        <v>30</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 09:32:21</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C85" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D85" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E85" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F85" s="15" t="n">
+        <v>61</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 09:32:21</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C86" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D86" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E86" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F86" s="15" t="n">
+        <v>132</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 09:32:21</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C87" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D87" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E87" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F87" s="15" t="n">
+        <v>191</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 09:32:21</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C88" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D88" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E88" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F88" s="14" t="n">
+        <v>30</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 09:32:21</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C89" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D89" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E89" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F89" s="15" t="n">
+        <v>516</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-19 09:32:21</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C90" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D90" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E90" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F90" s="15" t="n">
+        <v>75</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-20 09:09
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3883,6 +3883,310 @@
         </is>
       </c>
       <c r="H90" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-20 09:09:27</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C91" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D91" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E91" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F91" s="15" t="n">
+        <v>114</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-20 09:09:27</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C92" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D92" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E92" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F92" s="14" t="n">
+        <v>31</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-20 09:09:27</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C93" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D93" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E93" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F93" s="15" t="n">
+        <v>62</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-20 09:09:27</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C94" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D94" s="14" t="n">
+        <v>599</v>
+      </c>
+      <c r="E94" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F94" s="15" t="n">
+        <v>132</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-20 09:09:27</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C95" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D95" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E95" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F95" s="15" t="n">
+        <v>192</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-20 09:09:27</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C96" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D96" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E96" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F96" s="14" t="n">
+        <v>31</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-20 09:09:27</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C97" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D97" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E97" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F97" s="15" t="n">
+        <v>517</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-20 09:09:27</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C98" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D98" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E98" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F98" s="15" t="n">
+        <v>76</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-21 07:54
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4187,6 +4187,310 @@
         </is>
       </c>
       <c r="H98" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-21 07:54:59</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C99" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D99" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E99" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F99" s="15" t="n">
+        <v>63</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-21 07:54:59</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C100" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D100" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E100" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F100" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-21 07:54:59</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C101" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D101" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E101" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F101" s="15" t="n">
+        <v>115</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-21 07:54:59</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C102" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D102" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E102" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F102" s="15" t="n">
+        <v>133</v>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-21 07:54:59</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C103" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D103" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E103" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F103" s="15" t="n">
+        <v>193</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-21 07:54:59</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C104" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D104" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E104" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F104" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-21 07:54:59</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C105" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D105" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E105" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F105" s="15" t="n">
+        <v>518</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-21 07:54:59</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C106" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D106" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E106" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F106" s="15" t="n">
+        <v>77</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 07:58
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4491,6 +4491,310 @@
         </is>
       </c>
       <c r="H106" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 07:58:35</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C107" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D107" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E107" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F107" s="15" t="n">
+        <v>64</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 07:58:35</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C108" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D108" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E108" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F108" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 07:58:35</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C109" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D109" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E109" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F109" s="15" t="n">
+        <v>116</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 07:58:35</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C110" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D110" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E110" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F110" s="15" t="n">
+        <v>134</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 07:58:35</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C111" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D111" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E111" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F111" s="15" t="n">
+        <v>194</v>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 07:58:35</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C112" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D112" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E112" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F112" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 07:58:35</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C113" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D113" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E113" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F113" s="15" t="n">
+        <v>519</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 07:58:35</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C114" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D114" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E114" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F114" s="15" t="n">
+        <v>78</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 11:36
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4795,6 +4795,310 @@
         </is>
       </c>
       <c r="H114" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 11:36:29</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C115" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D115" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E115" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F115" s="15" t="n">
+        <v>64</v>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 11:36:29</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C116" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D116" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E116" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F116" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 11:36:29</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C117" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D117" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E117" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F117" s="15" t="n">
+        <v>116</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 11:36:29</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C118" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D118" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E118" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F118" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 11:36:29</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C119" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D119" s="14" t="n">
+        <v>58640</v>
+      </c>
+      <c r="E119" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F119" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 11:36:29</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C120" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D120" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E120" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F120" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 11:36:29</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C121" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D121" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E121" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F121" s="15" t="n">
+        <v>519</v>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 11:36:29</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C122" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D122" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E122" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F122" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 12:16
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H122"/>
+  <dimension ref="A1:H130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5099,6 +5099,310 @@
         </is>
       </c>
       <c r="H122" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:16:18</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C123" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D123" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E123" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F123" s="15" t="n">
+        <v>64</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:16:18</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C124" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D124" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E124" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F124" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:16:18</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C125" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D125" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E125" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F125" s="15" t="n">
+        <v>116</v>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:16:18</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C126" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D126" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E126" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F126" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:16:18</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C127" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D127" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F127" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:16:18</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C128" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D128" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E128" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F128" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:16:18</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C129" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D129" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E129" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F129" s="15" t="n">
+        <v>519</v>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:16:18</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C130" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D130" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E130" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F130" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 12:34
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H130"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5403,6 +5403,310 @@
         </is>
       </c>
       <c r="H130" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:34:28</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C131" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D131" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E131" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F131" s="15" t="n">
+        <v>64</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:34:28</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C132" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D132" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E132" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F132" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:34:28</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C133" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D133" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E133" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F133" s="15" t="n">
+        <v>116</v>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:34:28</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C134" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D134" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E134" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F134" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:34:28</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C135" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D135" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E135" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F135" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:34:28</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C136" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D136" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E136" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F136" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:34:28</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C137" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D137" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E137" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F137" s="15" t="n">
+        <v>519</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:34:28</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C138" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D138" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E138" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F138" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 12:40
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H138"/>
+  <dimension ref="A1:H146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5707,6 +5707,310 @@
         </is>
       </c>
       <c r="H138" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:40:56</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C139" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D139" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E139" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F139" s="15" t="n">
+        <v>64</v>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:40:56</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C140" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D140" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E140" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F140" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:40:56</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C141" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D141" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E141" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F141" s="15" t="n">
+        <v>116</v>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:40:56</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C142" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D142" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E142" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F142" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:40:56</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C143" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D143" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F143" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:40:56</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C144" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D144" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E144" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F144" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:40:56</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C145" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D145" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E145" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F145" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 12:40:56</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C146" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D146" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E146" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F146" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 13:31
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H146"/>
+  <dimension ref="A1:H154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6011,6 +6011,310 @@
         </is>
       </c>
       <c r="H146" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 13:31:28</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C147" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D147" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E147" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F147" s="15" t="n">
+        <v>64</v>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 13:31:28</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C148" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D148" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E148" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F148" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 13:31:28</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C149" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D149" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E149" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F149" s="15" t="n">
+        <v>116</v>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 13:31:28</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C150" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D150" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E150" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F150" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 13:31:28</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C151" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D151" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E151" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F151" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 13:31:28</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C152" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D152" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E152" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F152" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 13:31:28</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C153" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D153" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E153" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F153" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 13:31:28</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C154" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D154" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E154" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F154" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 17:34
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H154"/>
+  <dimension ref="A1:H162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6315,6 +6315,310 @@
         </is>
       </c>
       <c r="H154" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:34:38</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C155" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D155" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E155" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F155" s="15" t="n">
+        <v>65</v>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:34:38</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C156" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D156" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E156" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F156" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:34:38</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C157" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D157" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E157" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F157" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:34:38</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C158" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D158" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E158" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F158" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:34:38</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C159" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D159" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E159" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F159" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:34:38</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C160" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D160" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E160" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F160" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:34:38</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C161" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D161" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E161" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F161" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:34:38</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C162" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D162" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E162" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F162" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 17:49
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:H170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6619,6 +6619,304 @@
         </is>
       </c>
       <c r="H162" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:49:12</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C163" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D163" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E163" s="14" t="inlineStr"/>
+      <c r="F163" s="14" t="inlineStr"/>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:49:12</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C164" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D164" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E164" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F164" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:49:12</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C165" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D165" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E165" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F165" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:49:12</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C166" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D166" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E166" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F166" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:49:12</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C167" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D167" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E167" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F167" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:49:12</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C168" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D168" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E168" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F168" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:49:12</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C169" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D169" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E169" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F169" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 17:49:12</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C170" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D170" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E170" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F170" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 18:30
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H170"/>
+  <dimension ref="A1:H178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6917,6 +6917,310 @@
         </is>
       </c>
       <c r="H170" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 18:30:06</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C171" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D171" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E171" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F171" s="15" t="n">
+        <v>65</v>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 18:30:06</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C172" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D172" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E172" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F172" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 18:30:06</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C173" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D173" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E173" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F173" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 18:30:06</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C174" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D174" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E174" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F174" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 18:30:06</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C175" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D175" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E175" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F175" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 18:30:06</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C176" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D176" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E176" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F176" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 18:30:06</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C177" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D177" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E177" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F177" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 18:30:06</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C178" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D178" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E178" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F178" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 20:47
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H178"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7221,6 +7221,310 @@
         </is>
       </c>
       <c r="H178" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:47:59</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C179" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D179" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E179" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F179" s="15" t="n">
+        <v>65</v>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:47:59</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C180" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D180" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E180" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F180" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:47:59</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C181" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D181" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E181" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F181" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:47:59</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C182" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D182" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E182" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F182" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:47:59</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C183" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D183" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F183" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:47:59</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C184" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D184" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E184" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F184" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:47:59</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C185" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D185" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E185" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F185" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:47:59</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C186" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D186" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E186" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F186" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 20:59
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H186"/>
+  <dimension ref="A1:H194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7525,6 +7525,310 @@
         </is>
       </c>
       <c r="H186" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:59:28</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C187" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D187" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E187" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F187" s="15" t="n">
+        <v>65</v>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:59:28</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C188" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D188" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E188" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F188" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:59:28</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C189" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D189" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E189" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F189" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:59:28</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C190" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D190" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E190" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F190" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:59:28</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C191" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D191" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E191" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F191" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:59:28</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C192" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D192" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E192" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F192" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:59:28</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C193" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D193" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E193" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F193" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 20:59:28</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C194" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D194" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E194" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F194" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 21:03
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H194"/>
+  <dimension ref="A1:H202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7829,6 +7829,310 @@
         </is>
       </c>
       <c r="H194" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:03:42</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C195" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D195" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E195" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F195" s="15" t="n">
+        <v>65</v>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:03:42</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C196" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D196" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E196" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F196" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:03:42</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C197" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D197" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E197" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F197" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:03:42</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C198" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D198" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E198" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F198" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:03:42</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C199" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D199" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E199" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F199" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:03:42</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C200" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D200" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E200" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F200" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:03:42</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C201" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D201" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E201" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F201" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:03:42</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C202" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D202" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E202" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F202" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-22 21:13
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H202"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8133,6 +8133,310 @@
         </is>
       </c>
       <c r="H202" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:13:07</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C203" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D203" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E203" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F203" s="15" t="n">
+        <v>65</v>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:13:07</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C204" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D204" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E204" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F204" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:13:07</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C205" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D205" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E205" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F205" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:13:07</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C206" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D206" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E206" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F206" s="15" t="n">
+        <v>135</v>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:13:07</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C207" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D207" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E207" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F207" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:13:07</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C208" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D208" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E208" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F208" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:13:07</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C209" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D209" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E209" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F209" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-22 21:13:07</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C210" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D210" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E210" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F210" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-23 09:40
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H210"/>
+  <dimension ref="A1:H218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8437,6 +8437,310 @@
         </is>
       </c>
       <c r="H210" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-23 09:40:00</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C211" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D211" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E211" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F211" s="15" t="n">
+        <v>65</v>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-23 09:40:00</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C212" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D212" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E212" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F212" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-23 09:40:00</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C213" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D213" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E213" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F213" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-23 09:40:00</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C214" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D214" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E214" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F214" s="15" t="n">
+        <v>136</v>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-23 09:40:00</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C215" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D215" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E215" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F215" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-23 09:40:00</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C216" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D216" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E216" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F216" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-23 09:40:00</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C217" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D217" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E217" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F217" s="15" t="n">
+        <v>520</v>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-23 09:40:00</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C218" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D218" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E218" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F218" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-24 09:38
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H218"/>
+  <dimension ref="A1:H226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8741,6 +8741,310 @@
         </is>
       </c>
       <c r="H218" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-24 09:38:34</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C219" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D219" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E219" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F219" s="15" t="n">
+        <v>66</v>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-24 09:38:34</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C220" s="13" t="inlineStr">
+        <is>
+          <t>Świeżo wykończone mieszkanie z dużym balkonem - Ponikwoda</t>
+        </is>
+      </c>
+      <c r="D220" s="14" t="n">
+        <v>2299</v>
+      </c>
+      <c r="E220" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F220" s="14" t="n">
+        <v>35</v>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR.html</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>swiezo-wykonczone-mieszkanie-z-duzym-balkonem-ponikwoda-CID3-ID1951OR</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-24 09:38:34</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C221" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D221" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E221" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F221" s="15" t="n">
+        <v>118</v>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-24 09:38:34</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C222" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D222" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E222" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F222" s="15" t="n">
+        <v>137</v>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-24 09:38:34</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C223" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D223" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E223" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F223" s="14" t="n">
+        <v>35</v>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-24 09:38:34</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C224" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D224" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E224" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F224" s="15" t="n">
+        <v>196</v>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-24 09:38:34</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C225" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D225" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E225" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F225" s="15" t="n">
+        <v>521</v>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-24 09:38:34</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C226" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D226" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E226" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F226" s="15" t="n">
+        <v>80</v>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-25 09:39
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H226"/>
+  <dimension ref="A1:H233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9045,6 +9045,272 @@
         </is>
       </c>
       <c r="H226" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-25 09:39:39</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C227" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D227" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E227" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F227" s="15" t="n">
+        <v>119</v>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-25 09:39:39</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C228" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D228" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E228" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F228" s="15" t="n">
+        <v>138</v>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-25 09:39:39</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C229" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D229" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E229" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F229" s="15" t="n">
+        <v>67</v>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-25 09:39:39</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C230" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D230" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E230" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F230" s="14" t="n">
+        <v>36</v>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-25 09:39:39</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C231" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D231" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E231" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F231" s="15" t="n">
+        <v>197</v>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-25 09:39:39</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C232" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D232" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E232" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F232" s="15" t="n">
+        <v>522</v>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-25 09:39:39</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C233" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D233" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E233" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F233" s="15" t="n">
+        <v>81</v>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-26 09:35
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -47,6 +47,11 @@
     </font>
     <font>
       <color rgb="00ff6b6b"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="0047ffa0"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -104,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -149,6 +154,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -517,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H233"/>
+  <dimension ref="A1:H242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9311,6 +9319,348 @@
         </is>
       </c>
       <c r="H233" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C234" s="13" t="inlineStr">
+        <is>
+          <t>Duży pokój z balkonem w 2pokojowym mieszkaniu blisko Politechniki</t>
+        </is>
+      </c>
+      <c r="D234" s="14" t="n">
+        <v>1665</v>
+      </c>
+      <c r="E234" s="14" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="F234" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/duzy-pokoj-z-balkonem-w-2pokojowym-mieszkaniu-blisko-politechniki-CID3-ID19xpQK.html</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>duzy-pokoj-z-balkonem-w-2pokojowym-mieszkaniu-blisko-politechniki-CID3-ID19xpQK</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C235" s="13" t="inlineStr">
+        <is>
+          <t>Nowoczesne mieszkanie 2-pokojowe z balkonem, blisko UMCS, KUL, UP</t>
+        </is>
+      </c>
+      <c r="D235" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E235" s="14" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="F235" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/nowoczesne-mieszkanie-2-pokojowe-z-balkonem-blisko-umcs-kul-up-CID3-ID19xpwN.html</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>nowoczesne-mieszkanie-2-pokojowe-z-balkonem-blisko-umcs-kul-up-CID3-ID19xpwN</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C236" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D236" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E236" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F236" s="15" t="n">
+        <v>120</v>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C237" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D237" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E237" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F237" s="15" t="n">
+        <v>139</v>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C238" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D238" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E238" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F238" s="15" t="n">
+        <v>68</v>
+      </c>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C239" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D239" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E239" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F239" s="15" t="n">
+        <v>198</v>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C240" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D240" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E240" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F240" s="14" t="n">
+        <v>37</v>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C241" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D241" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E241" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F241" s="15" t="n">
+        <v>523</v>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-26 09:35:23</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C242" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D242" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E242" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F242" s="15" t="n">
+        <v>82</v>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-27 09:08
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -525,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H242"/>
+  <dimension ref="A1:H251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9661,6 +9661,348 @@
         </is>
       </c>
       <c r="H242" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C243" s="13" t="inlineStr">
+        <is>
+          <t>Duży pokój z balkonem w 2pokojowym mieszkaniu blisko Politechniki</t>
+        </is>
+      </c>
+      <c r="D243" s="14" t="n">
+        <v>1665</v>
+      </c>
+      <c r="E243" s="14" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="F243" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/duzy-pokoj-z-balkonem-w-2pokojowym-mieszkaniu-blisko-politechniki-CID3-ID19xpQK.html</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>duzy-pokoj-z-balkonem-w-2pokojowym-mieszkaniu-blisko-politechniki-CID3-ID19xpQK</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C244" s="13" t="inlineStr">
+        <is>
+          <t>Nowoczesne mieszkanie 2-pokojowe z balkonem, blisko UMCS, KUL, UP</t>
+        </is>
+      </c>
+      <c r="D244" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E244" s="14" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="F244" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/nowoczesne-mieszkanie-2-pokojowe-z-balkonem-blisko-umcs-kul-up-CID3-ID19xpwN.html</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>nowoczesne-mieszkanie-2-pokojowe-z-balkonem-blisko-umcs-kul-up-CID3-ID19xpwN</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C245" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D245" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E245" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F245" s="15" t="n">
+        <v>121</v>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C246" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D246" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E246" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F246" s="15" t="n">
+        <v>139</v>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C247" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D247" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E247" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F247" s="15" t="n">
+        <v>69</v>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C248" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D248" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E248" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F248" s="14" t="n">
+        <v>38</v>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C249" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D249" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E249" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F249" s="15" t="n">
+        <v>199</v>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C250" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D250" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E250" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F250" s="15" t="n">
+        <v>524</v>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-27 09:08:20</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C251" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D251" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E251" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F251" s="15" t="n">
+        <v>83</v>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-02-28 07:48
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -525,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H251"/>
+  <dimension ref="A1:H260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10003,6 +10003,348 @@
         </is>
       </c>
       <c r="H251" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C252" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D252" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E252" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F252" s="15" t="n">
+        <v>122</v>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C253" s="13" t="inlineStr">
+        <is>
+          <t>Duży pokój z balkonem w 2pokojowym mieszkaniu blisko Politechniki</t>
+        </is>
+      </c>
+      <c r="D253" s="14" t="n">
+        <v>1665</v>
+      </c>
+      <c r="E253" s="14" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="F253" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/duzy-pokoj-z-balkonem-w-2pokojowym-mieszkaniu-blisko-politechniki-CID3-ID19xpQK.html</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>duzy-pokoj-z-balkonem-w-2pokojowym-mieszkaniu-blisko-politechniki-CID3-ID19xpQK</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C254" s="13" t="inlineStr">
+        <is>
+          <t>Nowoczesne mieszkanie 2-pokojowe z balkonem, blisko UMCS, KUL, UP</t>
+        </is>
+      </c>
+      <c r="D254" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E254" s="14" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="F254" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/nowoczesne-mieszkanie-2-pokojowe-z-balkonem-blisko-umcs-kul-up-CID3-ID19xpwN.html</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>nowoczesne-mieszkanie-2-pokojowe-z-balkonem-blisko-umcs-kul-up-CID3-ID19xpwN</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C255" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D255" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E255" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F255" s="15" t="n">
+        <v>140</v>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C256" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D256" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E256" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F256" s="15" t="n">
+        <v>70</v>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C257" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D257" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E257" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F257" s="14" t="n">
+        <v>39</v>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C258" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D258" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E258" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F258" s="15" t="n">
+        <v>200</v>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C259" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D259" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E259" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F259" s="15" t="n">
+        <v>525</v>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="13" t="inlineStr">
+        <is>
+          <t>2026-02-28 07:48:03</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C260" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D260" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E260" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F260" s="15" t="n">
+        <v>84</v>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>

<commit_message>
📊 OLX Monitor 2026-03-01 07:54
</commit_message>
<xml_diff>
--- a/data/olx_monitoring.xlsx
+++ b/data/olx_monitoring.xlsx
@@ -525,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H260"/>
+  <dimension ref="A1:H269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10345,6 +10345,348 @@
         </is>
       </c>
       <c r="H260" t="inlineStr">
+        <is>
+          <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C261" s="13" t="inlineStr">
+        <is>
+          <t>Kawalerka po remoncie z funkcjonalną antresolą - ul. Jana Sawy</t>
+        </is>
+      </c>
+      <c r="D261" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E261" s="14" t="inlineStr">
+        <is>
+          <t>28.10.2025</t>
+        </is>
+      </c>
+      <c r="F261" s="15" t="n">
+        <v>123</v>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger.html</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>kawalerka-po-remoncie-z-funkcjonalna-antresola-ul-jana-sawy-CID3-ID183ger</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C262" s="13" t="inlineStr">
+        <is>
+          <t>Duży pokój z balkonem w 2pokojowym mieszkaniu blisko Politechniki</t>
+        </is>
+      </c>
+      <c r="D262" s="14" t="n">
+        <v>1665</v>
+      </c>
+      <c r="E262" s="14" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="F262" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/duzy-pokoj-z-balkonem-w-2pokojowym-mieszkaniu-blisko-politechniki-CID3-ID19xpQK.html</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>duzy-pokoj-z-balkonem-w-2pokojowym-mieszkaniu-blisko-politechniki-CID3-ID19xpQK</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C263" s="13" t="inlineStr">
+        <is>
+          <t>Nowoczesne mieszkanie 2-pokojowe z balkonem, blisko UMCS, KUL, UP</t>
+        </is>
+      </c>
+      <c r="D263" s="14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="E263" s="14" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="F263" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/nowoczesne-mieszkanie-2-pokojowe-z-balkonem-blisko-umcs-kul-up-CID3-ID19xpwN.html</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>nowoczesne-mieszkanie-2-pokojowe-z-balkonem-blisko-umcs-kul-up-CID3-ID19xpwN</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C264" s="13" t="inlineStr">
+        <is>
+          <t>Przytulny pokój blisko Politechniki – ul. Przytulna</t>
+        </is>
+      </c>
+      <c r="D264" s="14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E264" s="14" t="inlineStr">
+        <is>
+          <t>10.10.2025</t>
+        </is>
+      </c>
+      <c r="F264" s="15" t="n">
+        <v>141</v>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz.html</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>przytulny-pokoj-blisko-politechniki-ul-przytulna-CID3-ID17NeTz</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>poqui</t>
+        </is>
+      </c>
+      <c r="C265" s="13" t="inlineStr">
+        <is>
+          <t>Mieszkanie z KLIMATYZACJĄ 5 minut od UMCS, UP, KUL - Długosza</t>
+        </is>
+      </c>
+      <c r="D265" s="14" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E265" s="14" t="inlineStr">
+        <is>
+          <t>19.12.2025</t>
+        </is>
+      </c>
+      <c r="F265" s="15" t="n">
+        <v>71</v>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc.html</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>mieszkanie-z-klimatyzacja-5-minut-od-umcs-up-kul-dlugosza-CID3-ID18KAEc</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C266" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Super lokalizacja, blisko centrum, ul. Paganiniego 12</t>
+        </is>
+      </c>
+      <c r="D266" s="14" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E266" s="14" t="inlineStr">
+        <is>
+          <t>19.01.2026</t>
+        </is>
+      </c>
+      <c r="F266" s="14" t="n">
+        <v>40</v>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc.html</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-super-lokalizacja-blisko-centrum-ul-paganiniego-12-CID3-ID195dLc</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>pokojewlublinie</t>
+        </is>
+      </c>
+      <c r="C267" s="13" t="inlineStr">
+        <is>
+          <t>WOLNY OD ZARAZ! Pokój jedynka, ul. Romanowskiego 58</t>
+        </is>
+      </c>
+      <c r="D267" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E267" s="14" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="F267" s="15" t="n">
+        <v>201</v>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm.html</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>wolny-od-zaraz-pokoj-jedynka-ul-romanowskiego-58-CID3-ID16ZeYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C268" s="13" t="inlineStr">
+        <is>
+          <t>Ładny pokój jednoosobowy. Wynajmę duży pokój w centrum. ul Niecała 4.</t>
+        </is>
+      </c>
+      <c r="D268" s="14" t="n">
+        <v>730</v>
+      </c>
+      <c r="E268" s="14" t="inlineStr">
+        <is>
+          <t>20.09.2024</t>
+        </is>
+      </c>
+      <c r="F268" s="15" t="n">
+        <v>526</v>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM.html</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>ladny-pokoj-jednoosobowy-wynajme-duzy-pokoj-w-centrum-ul-niecala-4-CID3-ID122jPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="13" t="inlineStr">
+        <is>
+          <t>2026-03-01 07:54:11</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>dawnypatron</t>
+        </is>
+      </c>
+      <c r="C269" s="13" t="inlineStr">
+        <is>
+          <t>Mam do wynajęcia pokój dla os. pracującej lub studenta. Narutowicza 14</t>
+        </is>
+      </c>
+      <c r="D269" s="14" t="n">
+        <v>14690</v>
+      </c>
+      <c r="E269" s="14" t="inlineStr">
+        <is>
+          <t>05.12.2025</t>
+        </is>
+      </c>
+      <c r="F269" s="15" t="n">
+        <v>85</v>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>https://www.olx.pl/d/oferta/mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv.html</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr">
         <is>
           <t>mam-do-wynajecia-pokoj-dla-os-pracujacej-lub-studenta-narutowicza-14-CID3-ID18ySfv</t>
         </is>

</xml_diff>